<commit_message>
Finally fixed issues leading to wrong house edge
</commit_message>
<xml_diff>
--- a/Strategies/strategy_dealer_H17.xlsx
+++ b/Strategies/strategy_dealer_H17.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4dee3fe07fcb0db/Documents/Georgia Tech/2021 Fall/ISyE6644/Blackjack Project/Strategies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:40009_{10FE83E8-D7A2-49D6-97EC-C8B18B22337F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C53CFEFE-5D4A-48AC-B32F-FFFD4BA9A8CC}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:40009_{10FE83E8-D7A2-49D6-97EC-C8B18B22337F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6BB0DFD-C2D6-4378-A1CB-F2115D5397D6}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3525" yWindow="3525" windowWidth="15390" windowHeight="9532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hard" sheetId="2" r:id="rId1"/>
     <sheet name="soft" sheetId="1" r:id="rId2"/>
+    <sheet name="split" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="14">
   <si>
     <t>Stand</t>
   </si>
@@ -60,6 +61,9 @@
   </si>
   <si>
     <t>Dealer11</t>
+  </si>
+  <si>
+    <t>No Split</t>
   </si>
 </sst>
 </file>
@@ -596,7 +600,21 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -622,6 +640,20 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1694,6 +1726,351 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K19">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Split">
+      <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="Double">
+      <formula>NOT(ISERROR(SEARCH("Double",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Stand">
+      <formula>NOT(ISERROR(SEARCH("Stand",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Hit">
+      <formula>NOT(ISERROR(SEARCH("Hit",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="B2:K9">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Split">
       <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
     </cfRule>
@@ -1711,12 +2088,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K9"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCAEFDB-9576-416D-A82D-DA180375E303}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1761,34 +2138,34 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -1796,34 +2173,34 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -1831,34 +2208,34 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -1866,34 +2243,34 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -1901,34 +2278,34 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -1936,34 +2313,34 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -1971,34 +2348,34 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K8" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
@@ -2006,50 +2383,121 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K9" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B2:K9">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Split">
-      <formula>NOT(ISERROR(SEARCH("Split",B2)))</formula>
+  <conditionalFormatting sqref="G2:K11">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="No Split">
+      <formula>NOT(ISERROR(SEARCH("No Split",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Double">
-      <formula>NOT(ISERROR(SEARCH("Double",B2)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Surrender">
+      <formula>NOT(ISERROR(SEARCH("Surrender",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Stand">
-      <formula>NOT(ISERROR(SEARCH("Stand",B2)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:F11">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No Split">
+      <formula>NOT(ISERROR(SEARCH("No Split",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Hit">
-      <formula>NOT(ISERROR(SEARCH("Hit",B2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Surrender">
+      <formula>NOT(ISERROR(SEARCH("Surrender",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>